<commit_message>
Update evaluation result plots
</commit_message>
<xml_diff>
--- a/evaluation/results/genetics/analyze/per_question_metrics.xlsx
+++ b/evaluation/results/genetics/analyze/per_question_metrics.xlsx
@@ -22,40 +22,40 @@
     <t>question_preview_</t>
   </si>
   <si>
-    <t>LightRAG_Rel</t>
-  </si>
-  <si>
-    <t>LightRAG_Fact-F1</t>
-  </si>
-  <si>
-    <t>LightRAG_Fact-Rec</t>
-  </si>
-  <si>
-    <t>LightRAG_SemSim</t>
-  </si>
-  <si>
-    <t>GraphRAG_Rel</t>
-  </si>
-  <si>
-    <t>GraphRAG_Fact-F1</t>
-  </si>
-  <si>
-    <t>GraphRAG_Fact-Rec</t>
-  </si>
-  <si>
-    <t>GraphRAG_SemSim</t>
-  </si>
-  <si>
-    <t>NaiveRAG_Rel</t>
-  </si>
-  <si>
-    <t>NaiveRAG_Fact-F1</t>
-  </si>
-  <si>
-    <t>NaiveRAG_Fact-Rec</t>
-  </si>
-  <si>
-    <t>NaiveRAG_SemSim</t>
+    <t>LightRAG_answer_relevancy</t>
+  </si>
+  <si>
+    <t>LightRAG_factual_correctness(mode=f1)</t>
+  </si>
+  <si>
+    <t>LightRAG_factual_correctness(mode=recall)</t>
+  </si>
+  <si>
+    <t>LightRAG_semantic_similarity</t>
+  </si>
+  <si>
+    <t>GraphRAG_answer_relevancy</t>
+  </si>
+  <si>
+    <t>GraphRAG_factual_correctness(mode=f1)</t>
+  </si>
+  <si>
+    <t>GraphRAG_factual_correctness(mode=recall)</t>
+  </si>
+  <si>
+    <t>GraphRAG_semantic_similarity</t>
+  </si>
+  <si>
+    <t>NaiveRAG_answer_relevancy</t>
+  </si>
+  <si>
+    <t>NaiveRAG_factual_correctness(mode=f1)</t>
+  </si>
+  <si>
+    <t>NaiveRAG_factual_correctness(mode=recall)</t>
+  </si>
+  <si>
+    <t>NaiveRAG_semantic_similarity</t>
   </si>
   <si>
     <t>Explain Griffith's transformation experiments. What did he conclude from them?</t>

</xml_diff>